<commit_message>
added new stuff, including stuff for the PHing experiment
</commit_message>
<xml_diff>
--- a/TMA_supra_Experiment Plan.xlsx
+++ b/TMA_supra_Experiment Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="1520" windowWidth="26880" windowHeight="21660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4480" yWindow="6680" windowWidth="26880" windowHeight="21660" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Jar Numbers" sheetId="1" r:id="rId1"/>
@@ -988,7 +988,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection sqref="A1:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2003,7 +2003,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="74" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="57" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2011,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2945,8 +2945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3530,6 +3530,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>